<commit_message>
changes to recruitment options for sharks and skates, time of spawn for most species
</commit_message>
<xml_diff>
--- a/BevertonHolt.xlsx
+++ b/BevertonHolt.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="493">
   <si>
     <t>BHalpha_MAK</t>
   </si>
@@ -915,18 +915,6 @@
     <t>OSH_Time_Spawn</t>
   </si>
   <si>
-    <t>##CEP_Time_Spawn</t>
-  </si>
-  <si>
-    <t>##jCEP_Time_Spawn</t>
-  </si>
-  <si>
-    <t>##PWN_Time_Spawn</t>
-  </si>
-  <si>
-    <t>##jPWN_Time_Spawn</t>
-  </si>
-  <si>
     <t>MAK_spawn_period</t>
   </si>
   <si>
@@ -1501,6 +1489,21 @@
   </si>
   <si>
     <t>rec end</t>
+  </si>
+  <si>
+    <t>larval period</t>
+  </si>
+  <si>
+    <t>Su</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>Sp</t>
   </si>
 </sst>
 </file>
@@ -1516,12 +1519,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1536,9 +1545,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5111,2203 +5121,2270 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N68"/>
+  <dimension ref="A1:P64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G1" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>488</v>
+      </c>
+      <c r="I1" t="s">
+        <v>422</v>
+      </c>
+      <c r="O1" t="s">
+        <v>486</v>
+      </c>
+      <c r="P1" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>489</v>
+      </c>
+      <c r="C2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D2" s="2">
+        <v>210</v>
+      </c>
+      <c r="F2" t="s">
+        <v>296</v>
+      </c>
+      <c r="G2">
+        <v>7</v>
+      </c>
+      <c r="I2" t="s">
+        <v>359</v>
+      </c>
+      <c r="J2">
+        <v>30</v>
+      </c>
+      <c r="L2" t="s">
+        <v>423</v>
+      </c>
+      <c r="M2">
+        <v>60</v>
+      </c>
+      <c r="O2">
+        <f>D2+G2+J2</f>
+        <v>247</v>
+      </c>
+      <c r="P2">
+        <f>O2+M2</f>
+        <v>307</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>490</v>
+      </c>
+      <c r="C3" t="s">
+        <v>234</v>
+      </c>
+      <c r="D3">
+        <v>290</v>
+      </c>
+      <c r="F3" t="s">
+        <v>297</v>
+      </c>
+      <c r="G3">
+        <v>7</v>
+      </c>
+      <c r="I3" t="s">
+        <v>360</v>
+      </c>
+      <c r="J3">
+        <v>30</v>
+      </c>
+      <c r="L3" t="s">
+        <v>424</v>
+      </c>
+      <c r="M3">
+        <v>60</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O64" si="0">D3+G3+J3</f>
+        <v>327</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P64" si="1">O3+M3</f>
+        <v>387</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>489</v>
+      </c>
+      <c r="C4" t="s">
+        <v>235</v>
+      </c>
+      <c r="D4" s="2">
+        <v>180</v>
+      </c>
+      <c r="F4" t="s">
+        <v>298</v>
+      </c>
+      <c r="G4">
+        <v>7</v>
+      </c>
+      <c r="I4" t="s">
+        <v>361</v>
+      </c>
+      <c r="J4">
+        <v>60</v>
+      </c>
+      <c r="L4" t="s">
+        <v>425</v>
+      </c>
+      <c r="M4">
+        <v>90</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="0"/>
+        <v>247</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="1"/>
+        <v>337</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>489</v>
+      </c>
+      <c r="C5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D5">
+        <v>180</v>
+      </c>
+      <c r="F5" t="s">
+        <v>299</v>
+      </c>
+      <c r="G5">
+        <v>7</v>
+      </c>
+      <c r="I5" t="s">
+        <v>362</v>
+      </c>
+      <c r="J5">
+        <v>30</v>
+      </c>
+      <c r="L5" t="s">
         <v>426</v>
       </c>
-      <c r="M1" t="s">
-        <v>490</v>
-      </c>
-      <c r="N1" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>233</v>
-      </c>
-      <c r="B2">
-        <v>270</v>
-      </c>
-      <c r="D2" t="s">
-        <v>300</v>
-      </c>
-      <c r="E2">
-        <v>7</v>
-      </c>
-      <c r="G2" t="s">
-        <v>363</v>
-      </c>
-      <c r="H2">
+      <c r="M5">
         <v>30</v>
       </c>
-      <c r="J2" t="s">
-        <v>427</v>
-      </c>
-      <c r="K2">
-        <v>60</v>
-      </c>
-      <c r="M2">
-        <f>B2+E2+H2</f>
-        <v>307</v>
-      </c>
-      <c r="N2">
-        <f>M2+K2</f>
-        <v>367</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>234</v>
-      </c>
-      <c r="B3">
-        <v>290</v>
-      </c>
-      <c r="D3" t="s">
-        <v>301</v>
-      </c>
-      <c r="E3">
-        <v>7</v>
-      </c>
-      <c r="G3" t="s">
-        <v>364</v>
-      </c>
-      <c r="H3">
-        <v>30</v>
-      </c>
-      <c r="J3" t="s">
-        <v>428</v>
-      </c>
-      <c r="K3">
-        <v>60</v>
-      </c>
-      <c r="M3">
-        <f t="shared" ref="M3:M64" si="0">B3+E3+H3</f>
-        <v>327</v>
-      </c>
-      <c r="N3">
-        <f t="shared" ref="N3:N64" si="1">M3+K3</f>
-        <v>387</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>235</v>
-      </c>
-      <c r="B4">
-        <v>50</v>
-      </c>
-      <c r="D4" t="s">
-        <v>302</v>
-      </c>
-      <c r="E4">
-        <v>7</v>
-      </c>
-      <c r="G4" t="s">
-        <v>365</v>
-      </c>
-      <c r="H4">
-        <v>60</v>
-      </c>
-      <c r="J4" t="s">
-        <v>429</v>
-      </c>
-      <c r="K4">
-        <v>90</v>
-      </c>
-      <c r="M4">
-        <f t="shared" si="0"/>
-        <v>117</v>
-      </c>
-      <c r="N4">
-        <f t="shared" si="1"/>
-        <v>207</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>236</v>
-      </c>
-      <c r="B5">
-        <v>180</v>
-      </c>
-      <c r="D5" t="s">
-        <v>303</v>
-      </c>
-      <c r="E5">
-        <v>7</v>
-      </c>
-      <c r="G5" t="s">
-        <v>366</v>
-      </c>
-      <c r="H5">
-        <v>30</v>
-      </c>
-      <c r="J5" t="s">
-        <v>430</v>
-      </c>
-      <c r="K5">
-        <v>30</v>
-      </c>
-      <c r="M5">
+      <c r="O5">
         <f t="shared" si="0"/>
         <v>217</v>
       </c>
-      <c r="N5">
+      <c r="P5">
         <f t="shared" si="1"/>
         <v>247</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>489</v>
+      </c>
+      <c r="C6" t="s">
         <v>237</v>
       </c>
-      <c r="B6">
+      <c r="D6" s="2">
+        <v>180</v>
+      </c>
+      <c r="F6" t="s">
+        <v>300</v>
+      </c>
+      <c r="G6">
+        <v>7</v>
+      </c>
+      <c r="I6" t="s">
+        <v>363</v>
+      </c>
+      <c r="J6">
+        <v>80</v>
+      </c>
+      <c r="L6" t="s">
+        <v>427</v>
+      </c>
+      <c r="M6">
+        <v>90</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="0"/>
+        <v>267</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="1"/>
+        <v>357</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>490</v>
+      </c>
+      <c r="C7" t="s">
+        <v>238</v>
+      </c>
+      <c r="D7" s="2">
+        <v>270</v>
+      </c>
+      <c r="F7" t="s">
+        <v>301</v>
+      </c>
+      <c r="G7">
+        <v>7</v>
+      </c>
+      <c r="I7" t="s">
+        <v>364</v>
+      </c>
+      <c r="J7">
+        <v>80</v>
+      </c>
+      <c r="L7" t="s">
+        <v>428</v>
+      </c>
+      <c r="M7">
+        <v>90</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="0"/>
+        <v>357</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="1"/>
+        <v>447</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>491</v>
+      </c>
+      <c r="C8" t="s">
+        <v>239</v>
+      </c>
+      <c r="D8">
         <v>1</v>
       </c>
-      <c r="D6" t="s">
-        <v>304</v>
-      </c>
-      <c r="E6">
+      <c r="F8" t="s">
+        <v>302</v>
+      </c>
+      <c r="G8">
         <v>7</v>
       </c>
-      <c r="G6" t="s">
-        <v>367</v>
-      </c>
-      <c r="H6">
+      <c r="I8" t="s">
+        <v>365</v>
+      </c>
+      <c r="J8">
         <v>80</v>
       </c>
-      <c r="J6" t="s">
-        <v>431</v>
-      </c>
-      <c r="K6">
+      <c r="L8" t="s">
+        <v>429</v>
+      </c>
+      <c r="M8">
         <v>90</v>
       </c>
-      <c r="M6">
+      <c r="O8">
         <f t="shared" si="0"/>
         <v>88</v>
       </c>
-      <c r="N6">
+      <c r="P8">
         <f t="shared" si="1"/>
         <v>178</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>238</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>492</v>
+      </c>
+      <c r="C9" t="s">
+        <v>240</v>
+      </c>
+      <c r="D9" s="2">
+        <v>100</v>
+      </c>
+      <c r="F9" t="s">
+        <v>303</v>
+      </c>
+      <c r="G9">
+        <v>7</v>
+      </c>
+      <c r="I9" t="s">
+        <v>366</v>
+      </c>
+      <c r="J9" s="2">
+        <v>80</v>
+      </c>
+      <c r="L9" t="s">
+        <v>430</v>
+      </c>
+      <c r="M9">
+        <v>90</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="0"/>
+        <v>187</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="1"/>
+        <v>277</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>241</v>
+      </c>
+      <c r="D10" s="2">
+        <v>180</v>
+      </c>
+      <c r="F10" t="s">
+        <v>304</v>
+      </c>
+      <c r="G10">
+        <v>7</v>
+      </c>
+      <c r="I10" t="s">
+        <v>367</v>
+      </c>
+      <c r="J10">
+        <v>80</v>
+      </c>
+      <c r="L10" t="s">
+        <v>431</v>
+      </c>
+      <c r="M10">
+        <v>90</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="0"/>
+        <v>267</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="1"/>
+        <v>357</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>492</v>
+      </c>
+      <c r="C11" t="s">
+        <v>242</v>
+      </c>
+      <c r="D11" s="2">
+        <v>100</v>
+      </c>
+      <c r="F11" t="s">
         <v>305</v>
       </c>
-      <c r="E7">
+      <c r="G11">
         <v>7</v>
       </c>
-      <c r="G7" t="s">
+      <c r="I11" t="s">
         <v>368</v>
       </c>
-      <c r="H7">
+      <c r="J11">
         <v>80</v>
       </c>
-      <c r="J7" t="s">
+      <c r="L11" t="s">
         <v>432</v>
       </c>
-      <c r="K7">
+      <c r="M11">
         <v>90</v>
       </c>
-      <c r="M7">
+      <c r="O11">
         <f t="shared" si="0"/>
-        <v>88</v>
-      </c>
-      <c r="N7">
+        <v>187</v>
+      </c>
+      <c r="P11">
         <f t="shared" si="1"/>
-        <v>178</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>239</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>489</v>
+      </c>
+      <c r="C12" t="s">
+        <v>243</v>
+      </c>
+      <c r="D12" s="2">
+        <v>180</v>
+      </c>
+      <c r="F12" t="s">
         <v>306</v>
       </c>
-      <c r="E8">
+      <c r="G12">
         <v>7</v>
       </c>
-      <c r="G8" t="s">
+      <c r="I12" t="s">
         <v>369</v>
       </c>
-      <c r="H8">
+      <c r="J12">
         <v>80</v>
       </c>
-      <c r="J8" t="s">
+      <c r="L12" t="s">
         <v>433</v>
       </c>
-      <c r="K8">
+      <c r="M12">
         <v>90</v>
       </c>
-      <c r="M8">
+      <c r="O12">
         <f t="shared" si="0"/>
-        <v>88</v>
-      </c>
-      <c r="N8">
+        <v>267</v>
+      </c>
+      <c r="P12">
         <f t="shared" si="1"/>
-        <v>178</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>240</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>489</v>
+      </c>
+      <c r="C13" t="s">
+        <v>244</v>
+      </c>
+      <c r="D13" s="2">
+        <v>180</v>
+      </c>
+      <c r="F13" t="s">
         <v>307</v>
       </c>
-      <c r="E9">
+      <c r="G13">
         <v>7</v>
       </c>
-      <c r="G9" t="s">
+      <c r="I13" t="s">
         <v>370</v>
       </c>
-      <c r="H9">
+      <c r="J13">
         <v>80</v>
       </c>
-      <c r="J9" t="s">
+      <c r="L13" t="s">
         <v>434</v>
       </c>
-      <c r="K9">
+      <c r="M13">
         <v>90</v>
       </c>
-      <c r="M9">
+      <c r="O13">
         <f t="shared" si="0"/>
-        <v>88</v>
-      </c>
-      <c r="N9">
+        <v>267</v>
+      </c>
+      <c r="P13">
         <f t="shared" si="1"/>
-        <v>178</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>241</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>489</v>
+      </c>
+      <c r="C14" t="s">
+        <v>245</v>
+      </c>
+      <c r="D14" s="2">
+        <v>180</v>
+      </c>
+      <c r="F14" t="s">
         <v>308</v>
       </c>
-      <c r="E10">
+      <c r="G14">
         <v>7</v>
       </c>
-      <c r="G10" t="s">
+      <c r="I14" t="s">
         <v>371</v>
       </c>
-      <c r="H10">
-        <v>80</v>
-      </c>
-      <c r="J10" t="s">
+      <c r="J14">
+        <v>180</v>
+      </c>
+      <c r="L14" t="s">
         <v>435</v>
       </c>
-      <c r="K10">
-        <v>90</v>
-      </c>
-      <c r="M10">
+      <c r="M14">
+        <v>60</v>
+      </c>
+      <c r="O14">
         <f t="shared" si="0"/>
-        <v>88</v>
-      </c>
-      <c r="N10">
+        <v>367</v>
+      </c>
+      <c r="P14">
         <f t="shared" si="1"/>
-        <v>178</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>242</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>246</v>
+      </c>
+      <c r="D15" s="2">
+        <v>180</v>
+      </c>
+      <c r="F15" t="s">
         <v>309</v>
       </c>
-      <c r="E11">
+      <c r="G15">
         <v>7</v>
       </c>
-      <c r="G11" t="s">
+      <c r="I15" t="s">
         <v>372</v>
       </c>
-      <c r="H11">
-        <v>80</v>
-      </c>
-      <c r="J11" t="s">
+      <c r="J15">
+        <v>180</v>
+      </c>
+      <c r="L15" t="s">
         <v>436</v>
       </c>
-      <c r="K11">
-        <v>90</v>
-      </c>
-      <c r="M11">
+      <c r="M15">
+        <v>60</v>
+      </c>
+      <c r="O15">
         <f t="shared" si="0"/>
-        <v>88</v>
-      </c>
-      <c r="N11">
+        <v>367</v>
+      </c>
+      <c r="P15">
         <f t="shared" si="1"/>
-        <v>178</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>243</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>247</v>
+      </c>
+      <c r="D16" s="2">
+        <v>180</v>
+      </c>
+      <c r="F16" t="s">
         <v>310</v>
       </c>
-      <c r="E12">
+      <c r="G16">
         <v>7</v>
       </c>
-      <c r="G12" t="s">
+      <c r="I16" t="s">
         <v>373</v>
       </c>
-      <c r="H12">
-        <v>80</v>
-      </c>
-      <c r="J12" t="s">
+      <c r="J16">
+        <v>180</v>
+      </c>
+      <c r="L16" t="s">
         <v>437</v>
       </c>
-      <c r="K12">
-        <v>90</v>
-      </c>
-      <c r="M12">
+      <c r="M16">
+        <v>60</v>
+      </c>
+      <c r="O16">
         <f t="shared" si="0"/>
-        <v>88</v>
-      </c>
-      <c r="N12">
+        <v>367</v>
+      </c>
+      <c r="P16">
         <f t="shared" si="1"/>
-        <v>178</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>244</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>248</v>
+      </c>
+      <c r="D17">
+        <v>180</v>
+      </c>
+      <c r="F17" t="s">
         <v>311</v>
       </c>
-      <c r="E13">
+      <c r="G17">
         <v>7</v>
       </c>
-      <c r="G13" t="s">
+      <c r="I17" t="s">
         <v>374</v>
       </c>
-      <c r="H13">
-        <v>80</v>
-      </c>
-      <c r="J13" t="s">
+      <c r="J17">
+        <v>25</v>
+      </c>
+      <c r="L17" t="s">
         <v>438</v>
       </c>
-      <c r="K13">
-        <v>90</v>
-      </c>
-      <c r="M13">
-        <f t="shared" si="0"/>
-        <v>88</v>
-      </c>
-      <c r="N13">
-        <f t="shared" si="1"/>
-        <v>178</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>245</v>
-      </c>
-      <c r="B14">
-        <v>280</v>
-      </c>
-      <c r="D14" t="s">
-        <v>312</v>
-      </c>
-      <c r="E14">
-        <v>7</v>
-      </c>
-      <c r="G14" t="s">
-        <v>375</v>
-      </c>
-      <c r="H14">
-        <v>180</v>
-      </c>
-      <c r="J14" t="s">
-        <v>439</v>
-      </c>
-      <c r="K14">
-        <v>60</v>
-      </c>
-      <c r="M14">
-        <f t="shared" si="0"/>
-        <v>467</v>
-      </c>
-      <c r="N14">
-        <f t="shared" si="1"/>
-        <v>527</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>246</v>
-      </c>
-      <c r="B15">
-        <v>280</v>
-      </c>
-      <c r="D15" t="s">
-        <v>313</v>
-      </c>
-      <c r="E15">
-        <v>7</v>
-      </c>
-      <c r="G15" t="s">
-        <v>376</v>
-      </c>
-      <c r="H15">
-        <v>180</v>
-      </c>
-      <c r="J15" t="s">
-        <v>440</v>
-      </c>
-      <c r="K15">
-        <v>60</v>
-      </c>
-      <c r="M15">
-        <f t="shared" si="0"/>
-        <v>467</v>
-      </c>
-      <c r="N15">
-        <f t="shared" si="1"/>
-        <v>527</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>247</v>
-      </c>
-      <c r="B16">
-        <v>280</v>
-      </c>
-      <c r="D16" t="s">
-        <v>314</v>
-      </c>
-      <c r="E16">
-        <v>7</v>
-      </c>
-      <c r="G16" t="s">
-        <v>377</v>
-      </c>
-      <c r="H16">
-        <v>180</v>
-      </c>
-      <c r="J16" t="s">
-        <v>441</v>
-      </c>
-      <c r="K16">
-        <v>60</v>
-      </c>
-      <c r="M16">
-        <f t="shared" si="0"/>
-        <v>467</v>
-      </c>
-      <c r="N16">
-        <f t="shared" si="1"/>
-        <v>527</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>248</v>
-      </c>
-      <c r="B17">
-        <v>180</v>
-      </c>
-      <c r="D17" t="s">
-        <v>315</v>
-      </c>
-      <c r="E17">
-        <v>7</v>
-      </c>
-      <c r="G17" t="s">
-        <v>378</v>
-      </c>
-      <c r="H17">
-        <v>25</v>
-      </c>
-      <c r="J17" t="s">
-        <v>442</v>
-      </c>
-      <c r="K17">
+      <c r="M17">
         <v>30</v>
       </c>
-      <c r="M17">
+      <c r="O17">
         <f t="shared" si="0"/>
         <v>212</v>
       </c>
-      <c r="N17">
+      <c r="P17">
         <f t="shared" si="1"/>
         <v>242</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>489</v>
+      </c>
+      <c r="C18" t="s">
         <v>249</v>
       </c>
-      <c r="B18">
+      <c r="D18">
         <v>100</v>
       </c>
-      <c r="D18" t="s">
-        <v>316</v>
-      </c>
-      <c r="E18">
+      <c r="F18" t="s">
+        <v>312</v>
+      </c>
+      <c r="G18">
         <v>7</v>
       </c>
-      <c r="G18" t="s">
-        <v>379</v>
-      </c>
-      <c r="H18">
+      <c r="I18" t="s">
+        <v>375</v>
+      </c>
+      <c r="J18">
         <v>35</v>
       </c>
-      <c r="J18" t="s">
-        <v>443</v>
-      </c>
-      <c r="K18">
+      <c r="L18" t="s">
+        <v>439</v>
+      </c>
+      <c r="M18">
         <v>40</v>
       </c>
-      <c r="M18">
+      <c r="O18">
         <f t="shared" si="0"/>
         <v>142</v>
       </c>
-      <c r="N18">
+      <c r="P18">
         <f t="shared" si="1"/>
         <v>182</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
         <v>250</v>
       </c>
-      <c r="B19">
+      <c r="D19">
         <v>100</v>
       </c>
-      <c r="D19" t="s">
-        <v>317</v>
-      </c>
-      <c r="E19">
+      <c r="F19" t="s">
+        <v>313</v>
+      </c>
+      <c r="G19">
         <v>7</v>
       </c>
-      <c r="G19" t="s">
-        <v>380</v>
-      </c>
-      <c r="H19">
+      <c r="I19" t="s">
+        <v>376</v>
+      </c>
+      <c r="J19">
         <v>35</v>
       </c>
-      <c r="J19" t="s">
-        <v>444</v>
-      </c>
-      <c r="K19">
+      <c r="L19" t="s">
+        <v>440</v>
+      </c>
+      <c r="M19">
         <v>40</v>
       </c>
-      <c r="M19">
+      <c r="O19">
         <f t="shared" si="0"/>
         <v>142</v>
       </c>
-      <c r="N19">
+      <c r="P19">
         <f t="shared" si="1"/>
         <v>182</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
         <v>251</v>
       </c>
-      <c r="B20">
+      <c r="D20">
         <v>100</v>
       </c>
-      <c r="D20" t="s">
-        <v>318</v>
-      </c>
-      <c r="E20">
+      <c r="F20" t="s">
+        <v>314</v>
+      </c>
+      <c r="G20">
         <v>7</v>
       </c>
-      <c r="G20" t="s">
-        <v>381</v>
-      </c>
-      <c r="H20">
+      <c r="I20" t="s">
+        <v>377</v>
+      </c>
+      <c r="J20">
         <v>35</v>
       </c>
-      <c r="J20" t="s">
-        <v>445</v>
-      </c>
-      <c r="K20">
+      <c r="L20" t="s">
+        <v>441</v>
+      </c>
+      <c r="M20">
         <v>40</v>
       </c>
-      <c r="M20">
+      <c r="O20">
         <f t="shared" si="0"/>
         <v>142</v>
       </c>
-      <c r="N20">
+      <c r="P20">
         <f t="shared" si="1"/>
         <v>182</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>489</v>
+      </c>
+      <c r="C21" t="s">
         <v>252</v>
       </c>
-      <c r="B21">
+      <c r="D21" s="2">
+        <v>180</v>
+      </c>
+      <c r="F21" t="s">
+        <v>315</v>
+      </c>
+      <c r="G21">
+        <v>7</v>
+      </c>
+      <c r="I21" t="s">
+        <v>378</v>
+      </c>
+      <c r="J21">
+        <v>60</v>
+      </c>
+      <c r="L21" t="s">
+        <v>442</v>
+      </c>
+      <c r="M21">
+        <v>60</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="0"/>
+        <v>247</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="1"/>
+        <v>307</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>490</v>
+      </c>
+      <c r="C22" t="s">
+        <v>253</v>
+      </c>
+      <c r="D22" s="2">
         <v>270</v>
       </c>
-      <c r="D21" t="s">
+      <c r="F22" t="s">
+        <v>316</v>
+      </c>
+      <c r="G22">
+        <v>7</v>
+      </c>
+      <c r="I22" t="s">
+        <v>379</v>
+      </c>
+      <c r="J22">
+        <v>30</v>
+      </c>
+      <c r="L22" t="s">
+        <v>443</v>
+      </c>
+      <c r="M22">
+        <v>40</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="0"/>
+        <v>307</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="1"/>
+        <v>347</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>254</v>
+      </c>
+      <c r="D23">
+        <v>10</v>
+      </c>
+      <c r="F23" t="s">
+        <v>317</v>
+      </c>
+      <c r="G23">
+        <v>7</v>
+      </c>
+      <c r="I23" t="s">
+        <v>380</v>
+      </c>
+      <c r="J23">
+        <v>30</v>
+      </c>
+      <c r="L23" t="s">
+        <v>444</v>
+      </c>
+      <c r="M23">
+        <v>40</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>491</v>
+      </c>
+      <c r="C24" t="s">
+        <v>255</v>
+      </c>
+      <c r="D24">
+        <v>20</v>
+      </c>
+      <c r="F24" t="s">
+        <v>318</v>
+      </c>
+      <c r="G24">
+        <v>7</v>
+      </c>
+      <c r="I24" t="s">
+        <v>381</v>
+      </c>
+      <c r="J24">
+        <v>60</v>
+      </c>
+      <c r="L24" t="s">
+        <v>445</v>
+      </c>
+      <c r="M24">
+        <v>90</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="0"/>
+        <v>87</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="1"/>
+        <v>177</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>489</v>
+      </c>
+      <c r="C25" t="s">
+        <v>256</v>
+      </c>
+      <c r="D25" s="2">
+        <v>150</v>
+      </c>
+      <c r="F25" t="s">
         <v>319</v>
       </c>
-      <c r="E21">
+      <c r="G25">
         <v>7</v>
       </c>
-      <c r="G21" t="s">
+      <c r="I25" t="s">
         <v>382</v>
       </c>
-      <c r="H21">
+      <c r="J25">
+        <v>30</v>
+      </c>
+      <c r="L25" t="s">
+        <v>446</v>
+      </c>
+      <c r="M25">
+        <v>90</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="0"/>
+        <v>187</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="1"/>
+        <v>277</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>489</v>
+      </c>
+      <c r="C26" t="s">
+        <v>257</v>
+      </c>
+      <c r="D26" s="2">
+        <v>150</v>
+      </c>
+      <c r="F26" t="s">
+        <v>320</v>
+      </c>
+      <c r="G26">
+        <v>7</v>
+      </c>
+      <c r="I26" t="s">
+        <v>383</v>
+      </c>
+      <c r="J26">
+        <v>30</v>
+      </c>
+      <c r="L26" t="s">
+        <v>447</v>
+      </c>
+      <c r="M26">
+        <v>90</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="0"/>
+        <v>187</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="1"/>
+        <v>277</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>491</v>
+      </c>
+      <c r="C27" t="s">
+        <v>258</v>
+      </c>
+      <c r="D27">
+        <v>10</v>
+      </c>
+      <c r="F27" t="s">
+        <v>321</v>
+      </c>
+      <c r="G27">
+        <v>7</v>
+      </c>
+      <c r="I27" t="s">
+        <v>384</v>
+      </c>
+      <c r="J27">
+        <v>30</v>
+      </c>
+      <c r="L27" t="s">
+        <v>448</v>
+      </c>
+      <c r="M27">
+        <v>90</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="1"/>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>489</v>
+      </c>
+      <c r="C28" t="s">
+        <v>259</v>
+      </c>
+      <c r="D28" s="2">
+        <v>180</v>
+      </c>
+      <c r="F28" t="s">
+        <v>322</v>
+      </c>
+      <c r="G28">
+        <v>7</v>
+      </c>
+      <c r="I28" t="s">
+        <v>385</v>
+      </c>
+      <c r="J28">
+        <v>30</v>
+      </c>
+      <c r="L28" t="s">
+        <v>449</v>
+      </c>
+      <c r="M28">
+        <v>90</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="0"/>
+        <v>217</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="1"/>
+        <v>307</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>489</v>
+      </c>
+      <c r="C29" t="s">
+        <v>260</v>
+      </c>
+      <c r="D29" s="2">
+        <v>150</v>
+      </c>
+      <c r="F29" t="s">
+        <v>323</v>
+      </c>
+      <c r="G29">
+        <v>7</v>
+      </c>
+      <c r="I29" t="s">
+        <v>386</v>
+      </c>
+      <c r="J29">
+        <v>30</v>
+      </c>
+      <c r="L29" t="s">
+        <v>450</v>
+      </c>
+      <c r="M29">
+        <v>90</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="0"/>
+        <v>187</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="1"/>
+        <v>277</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>489</v>
+      </c>
+      <c r="C30" t="s">
+        <v>261</v>
+      </c>
+      <c r="D30" s="2">
+        <v>150</v>
+      </c>
+      <c r="F30" t="s">
+        <v>324</v>
+      </c>
+      <c r="G30">
+        <v>7</v>
+      </c>
+      <c r="I30" t="s">
+        <v>387</v>
+      </c>
+      <c r="J30">
+        <v>30</v>
+      </c>
+      <c r="L30" t="s">
+        <v>451</v>
+      </c>
+      <c r="M30">
+        <v>90</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="0"/>
+        <v>187</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="1"/>
+        <v>277</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>262</v>
+      </c>
+      <c r="D31">
+        <v>10</v>
+      </c>
+      <c r="F31" t="s">
+        <v>325</v>
+      </c>
+      <c r="G31">
+        <v>7</v>
+      </c>
+      <c r="I31" t="s">
+        <v>388</v>
+      </c>
+      <c r="J31">
+        <v>30</v>
+      </c>
+      <c r="L31" t="s">
+        <v>452</v>
+      </c>
+      <c r="M31">
+        <v>90</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="1"/>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>492</v>
+      </c>
+      <c r="C32" t="s">
+        <v>263</v>
+      </c>
+      <c r="D32" s="2">
+        <v>100</v>
+      </c>
+      <c r="F32" t="s">
+        <v>326</v>
+      </c>
+      <c r="G32">
+        <v>7</v>
+      </c>
+      <c r="I32" t="s">
+        <v>389</v>
+      </c>
+      <c r="J32">
+        <v>30</v>
+      </c>
+      <c r="L32" t="s">
+        <v>453</v>
+      </c>
+      <c r="M32">
+        <v>90</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="0"/>
+        <v>137</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="1"/>
+        <v>227</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>264</v>
+      </c>
+      <c r="D33" s="2">
+        <v>100</v>
+      </c>
+      <c r="F33" t="s">
+        <v>327</v>
+      </c>
+      <c r="G33">
+        <v>7</v>
+      </c>
+      <c r="I33" t="s">
+        <v>390</v>
+      </c>
+      <c r="J33">
+        <v>30</v>
+      </c>
+      <c r="L33" t="s">
+        <v>454</v>
+      </c>
+      <c r="M33">
+        <v>90</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="0"/>
+        <v>137</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="1"/>
+        <v>227</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>265</v>
+      </c>
+      <c r="D34" s="2">
+        <v>220</v>
+      </c>
+      <c r="F34" t="s">
+        <v>328</v>
+      </c>
+      <c r="G34">
+        <v>7</v>
+      </c>
+      <c r="I34" t="s">
+        <v>391</v>
+      </c>
+      <c r="J34">
+        <v>30</v>
+      </c>
+      <c r="L34" t="s">
+        <v>455</v>
+      </c>
+      <c r="M34">
+        <v>90</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="0"/>
+        <v>257</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="1"/>
+        <v>347</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>489</v>
+      </c>
+      <c r="C35" t="s">
+        <v>266</v>
+      </c>
+      <c r="D35" s="2">
+        <v>180</v>
+      </c>
+      <c r="F35" t="s">
+        <v>329</v>
+      </c>
+      <c r="G35">
+        <v>7</v>
+      </c>
+      <c r="I35" t="s">
+        <v>392</v>
+      </c>
+      <c r="J35">
+        <v>30</v>
+      </c>
+      <c r="L35" t="s">
+        <v>456</v>
+      </c>
+      <c r="M35">
+        <v>90</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="0"/>
+        <v>217</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="1"/>
+        <v>307</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>489</v>
+      </c>
+      <c r="C36" t="s">
+        <v>267</v>
+      </c>
+      <c r="D36" s="2">
+        <v>180</v>
+      </c>
+      <c r="F36" t="s">
+        <v>330</v>
+      </c>
+      <c r="G36">
+        <v>7</v>
+      </c>
+      <c r="I36" t="s">
+        <v>393</v>
+      </c>
+      <c r="J36">
+        <v>30</v>
+      </c>
+      <c r="L36" t="s">
+        <v>457</v>
+      </c>
+      <c r="M36">
+        <v>90</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="0"/>
+        <v>217</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="1"/>
+        <v>307</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>489</v>
+      </c>
+      <c r="C37" t="s">
+        <v>268</v>
+      </c>
+      <c r="D37" s="2">
+        <v>180</v>
+      </c>
+      <c r="F37" t="s">
+        <v>331</v>
+      </c>
+      <c r="G37">
+        <v>7</v>
+      </c>
+      <c r="I37" t="s">
+        <v>394</v>
+      </c>
+      <c r="J37">
+        <v>30</v>
+      </c>
+      <c r="L37" t="s">
+        <v>458</v>
+      </c>
+      <c r="M37">
+        <v>90</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="0"/>
+        <v>217</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="1"/>
+        <v>307</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>491</v>
+      </c>
+      <c r="C38" t="s">
+        <v>269</v>
+      </c>
+      <c r="D38">
+        <v>10</v>
+      </c>
+      <c r="F38" t="s">
+        <v>332</v>
+      </c>
+      <c r="G38">
+        <v>7</v>
+      </c>
+      <c r="I38" t="s">
+        <v>395</v>
+      </c>
+      <c r="J38">
+        <v>30</v>
+      </c>
+      <c r="L38" t="s">
+        <v>459</v>
+      </c>
+      <c r="M38">
+        <v>90</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="1"/>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>270</v>
+      </c>
+      <c r="D39">
+        <v>10</v>
+      </c>
+      <c r="F39" t="s">
+        <v>333</v>
+      </c>
+      <c r="G39">
+        <v>7</v>
+      </c>
+      <c r="I39" t="s">
+        <v>396</v>
+      </c>
+      <c r="J39">
+        <v>30</v>
+      </c>
+      <c r="L39" t="s">
+        <v>460</v>
+      </c>
+      <c r="M39">
+        <v>90</v>
+      </c>
+      <c r="O39">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="1"/>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>271</v>
+      </c>
+      <c r="D40">
+        <v>10</v>
+      </c>
+      <c r="F40" t="s">
+        <v>334</v>
+      </c>
+      <c r="G40">
+        <v>7</v>
+      </c>
+      <c r="I40" t="s">
+        <v>397</v>
+      </c>
+      <c r="J40">
+        <v>30</v>
+      </c>
+      <c r="L40" t="s">
+        <v>461</v>
+      </c>
+      <c r="M40">
+        <v>90</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="1"/>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>491</v>
+      </c>
+      <c r="C41" t="s">
+        <v>272</v>
+      </c>
+      <c r="D41">
+        <v>30</v>
+      </c>
+      <c r="F41" t="s">
+        <v>335</v>
+      </c>
+      <c r="G41">
+        <v>7</v>
+      </c>
+      <c r="I41" t="s">
+        <v>398</v>
+      </c>
+      <c r="J41">
+        <v>30</v>
+      </c>
+      <c r="L41" t="s">
+        <v>462</v>
+      </c>
+      <c r="M41">
+        <v>90</v>
+      </c>
+      <c r="O41">
+        <f t="shared" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="P41">
+        <f t="shared" si="1"/>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>492</v>
+      </c>
+      <c r="C42" t="s">
+        <v>273</v>
+      </c>
+      <c r="D42">
         <v>60</v>
       </c>
-      <c r="J21" t="s">
-        <v>446</v>
-      </c>
-      <c r="K21">
+      <c r="F42" t="s">
+        <v>336</v>
+      </c>
+      <c r="G42">
+        <v>7</v>
+      </c>
+      <c r="I42" t="s">
+        <v>399</v>
+      </c>
+      <c r="J42">
+        <v>40</v>
+      </c>
+      <c r="L42" t="s">
+        <v>463</v>
+      </c>
+      <c r="M42">
+        <v>90</v>
+      </c>
+      <c r="O42">
+        <f t="shared" si="0"/>
+        <v>107</v>
+      </c>
+      <c r="P42">
+        <f t="shared" si="1"/>
+        <v>197</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>274</v>
+      </c>
+      <c r="D43" s="2">
+        <v>180</v>
+      </c>
+      <c r="F43" t="s">
+        <v>337</v>
+      </c>
+      <c r="G43">
+        <v>7</v>
+      </c>
+      <c r="I43" t="s">
+        <v>400</v>
+      </c>
+      <c r="J43">
+        <v>270</v>
+      </c>
+      <c r="L43" t="s">
+        <v>464</v>
+      </c>
+      <c r="M43">
+        <v>90</v>
+      </c>
+      <c r="O43">
+        <f t="shared" si="0"/>
+        <v>457</v>
+      </c>
+      <c r="P43">
+        <f t="shared" si="1"/>
+        <v>547</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>275</v>
+      </c>
+      <c r="D44">
+        <v>160</v>
+      </c>
+      <c r="F44" t="s">
+        <v>338</v>
+      </c>
+      <c r="G44">
+        <v>7</v>
+      </c>
+      <c r="I44" t="s">
+        <v>401</v>
+      </c>
+      <c r="J44">
+        <v>360</v>
+      </c>
+      <c r="L44" t="s">
+        <v>465</v>
+      </c>
+      <c r="M44">
+        <v>90</v>
+      </c>
+      <c r="O44">
+        <f t="shared" si="0"/>
+        <v>527</v>
+      </c>
+      <c r="P44">
+        <f t="shared" si="1"/>
+        <v>617</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>276</v>
+      </c>
+      <c r="D45">
+        <v>160</v>
+      </c>
+      <c r="F45" t="s">
+        <v>339</v>
+      </c>
+      <c r="G45">
+        <v>7</v>
+      </c>
+      <c r="I45" t="s">
+        <v>402</v>
+      </c>
+      <c r="J45">
+        <v>360</v>
+      </c>
+      <c r="L45" t="s">
+        <v>466</v>
+      </c>
+      <c r="M45">
+        <v>90</v>
+      </c>
+      <c r="O45">
+        <f t="shared" si="0"/>
+        <v>527</v>
+      </c>
+      <c r="P45">
+        <f t="shared" si="1"/>
+        <v>617</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>277</v>
+      </c>
+      <c r="D46">
+        <v>160</v>
+      </c>
+      <c r="F46" t="s">
+        <v>340</v>
+      </c>
+      <c r="G46">
+        <v>7</v>
+      </c>
+      <c r="I46" t="s">
+        <v>403</v>
+      </c>
+      <c r="J46">
+        <v>360</v>
+      </c>
+      <c r="L46" t="s">
+        <v>467</v>
+      </c>
+      <c r="M46">
+        <v>90</v>
+      </c>
+      <c r="O46">
+        <f t="shared" si="0"/>
+        <v>527</v>
+      </c>
+      <c r="P46">
+        <f t="shared" si="1"/>
+        <v>617</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>278</v>
+      </c>
+      <c r="D47">
+        <v>150</v>
+      </c>
+      <c r="F47" t="s">
+        <v>341</v>
+      </c>
+      <c r="G47">
+        <v>7</v>
+      </c>
+      <c r="I47" t="s">
+        <v>404</v>
+      </c>
+      <c r="J47">
+        <v>360</v>
+      </c>
+      <c r="L47" t="s">
+        <v>468</v>
+      </c>
+      <c r="M47">
+        <v>40</v>
+      </c>
+      <c r="O47">
+        <f t="shared" si="0"/>
+        <v>517</v>
+      </c>
+      <c r="P47">
+        <f t="shared" si="1"/>
+        <v>557</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>279</v>
+      </c>
+      <c r="D48">
+        <v>150</v>
+      </c>
+      <c r="F48" t="s">
+        <v>342</v>
+      </c>
+      <c r="G48">
+        <v>7</v>
+      </c>
+      <c r="I48" t="s">
+        <v>405</v>
+      </c>
+      <c r="J48">
+        <v>360</v>
+      </c>
+      <c r="L48" t="s">
+        <v>469</v>
+      </c>
+      <c r="M48">
+        <v>40</v>
+      </c>
+      <c r="O48">
+        <f t="shared" si="0"/>
+        <v>517</v>
+      </c>
+      <c r="P48">
+        <f t="shared" si="1"/>
+        <v>557</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>280</v>
+      </c>
+      <c r="D49">
+        <v>150</v>
+      </c>
+      <c r="F49" t="s">
+        <v>343</v>
+      </c>
+      <c r="G49">
+        <v>7</v>
+      </c>
+      <c r="I49" t="s">
+        <v>406</v>
+      </c>
+      <c r="J49">
+        <v>360</v>
+      </c>
+      <c r="L49" t="s">
+        <v>470</v>
+      </c>
+      <c r="M49">
+        <v>40</v>
+      </c>
+      <c r="O49">
+        <f t="shared" si="0"/>
+        <v>517</v>
+      </c>
+      <c r="P49">
+        <f t="shared" si="1"/>
+        <v>557</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>489</v>
+      </c>
+      <c r="C50" t="s">
+        <v>281</v>
+      </c>
+      <c r="D50" s="2">
+        <v>190</v>
+      </c>
+      <c r="F50" t="s">
+        <v>344</v>
+      </c>
+      <c r="G50" s="2">
+        <v>90</v>
+      </c>
+      <c r="I50" t="s">
+        <v>407</v>
+      </c>
+      <c r="J50" s="2">
+        <v>84</v>
+      </c>
+      <c r="L50" t="s">
+        <v>471</v>
+      </c>
+      <c r="M50">
+        <v>90</v>
+      </c>
+      <c r="O50">
+        <f t="shared" si="0"/>
+        <v>364</v>
+      </c>
+      <c r="P50">
+        <f t="shared" si="1"/>
+        <v>454</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>489</v>
+      </c>
+      <c r="C51" t="s">
+        <v>282</v>
+      </c>
+      <c r="D51" s="2">
+        <v>190</v>
+      </c>
+      <c r="F51" t="s">
+        <v>345</v>
+      </c>
+      <c r="G51" s="2">
+        <v>90</v>
+      </c>
+      <c r="I51" t="s">
+        <v>408</v>
+      </c>
+      <c r="J51" s="2">
+        <v>84</v>
+      </c>
+      <c r="L51" t="s">
+        <v>472</v>
+      </c>
+      <c r="M51">
+        <v>90</v>
+      </c>
+      <c r="O51">
+        <f t="shared" si="0"/>
+        <v>364</v>
+      </c>
+      <c r="P51">
+        <f t="shared" si="1"/>
+        <v>454</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>489</v>
+      </c>
+      <c r="C52" t="s">
+        <v>283</v>
+      </c>
+      <c r="D52" s="2">
+        <v>190</v>
+      </c>
+      <c r="F52" t="s">
+        <v>346</v>
+      </c>
+      <c r="G52" s="2">
+        <v>90</v>
+      </c>
+      <c r="I52" t="s">
+        <v>409</v>
+      </c>
+      <c r="J52" s="2">
+        <v>84</v>
+      </c>
+      <c r="L52" t="s">
+        <v>473</v>
+      </c>
+      <c r="M52">
+        <v>90</v>
+      </c>
+      <c r="O52">
+        <f t="shared" si="0"/>
+        <v>364</v>
+      </c>
+      <c r="P52">
+        <f t="shared" si="1"/>
+        <v>454</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>284</v>
+      </c>
+      <c r="D53">
+        <v>290</v>
+      </c>
+      <c r="F53" t="s">
+        <v>347</v>
+      </c>
+      <c r="G53">
+        <v>7</v>
+      </c>
+      <c r="I53" t="s">
+        <v>410</v>
+      </c>
+      <c r="J53">
+        <v>200</v>
+      </c>
+      <c r="L53" t="s">
+        <v>474</v>
+      </c>
+      <c r="M53">
+        <v>50</v>
+      </c>
+      <c r="O53">
+        <f t="shared" si="0"/>
+        <v>497</v>
+      </c>
+      <c r="P53">
+        <f t="shared" si="1"/>
+        <v>547</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>285</v>
+      </c>
+      <c r="D54">
+        <v>230</v>
+      </c>
+      <c r="F54" t="s">
+        <v>348</v>
+      </c>
+      <c r="G54">
+        <v>7</v>
+      </c>
+      <c r="I54" t="s">
+        <v>411</v>
+      </c>
+      <c r="J54">
+        <v>330</v>
+      </c>
+      <c r="L54" t="s">
+        <v>475</v>
+      </c>
+      <c r="M54">
+        <v>30</v>
+      </c>
+      <c r="O54">
+        <f t="shared" si="0"/>
+        <v>567</v>
+      </c>
+      <c r="P54">
+        <f t="shared" si="1"/>
+        <v>597</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>286</v>
+      </c>
+      <c r="D55">
+        <v>270</v>
+      </c>
+      <c r="F55" t="s">
+        <v>349</v>
+      </c>
+      <c r="G55">
+        <v>7</v>
+      </c>
+      <c r="I55" t="s">
+        <v>412</v>
+      </c>
+      <c r="J55">
+        <v>360</v>
+      </c>
+      <c r="L55" t="s">
+        <v>476</v>
+      </c>
+      <c r="M55">
         <v>60</v>
       </c>
-      <c r="M21">
+      <c r="O55">
+        <f t="shared" si="0"/>
+        <v>637</v>
+      </c>
+      <c r="P55">
+        <f t="shared" si="1"/>
+        <v>697</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>287</v>
+      </c>
+      <c r="D56">
+        <v>220</v>
+      </c>
+      <c r="F56" t="s">
+        <v>350</v>
+      </c>
+      <c r="G56">
+        <v>7</v>
+      </c>
+      <c r="I56" t="s">
+        <v>413</v>
+      </c>
+      <c r="J56">
+        <v>360</v>
+      </c>
+      <c r="L56" t="s">
+        <v>477</v>
+      </c>
+      <c r="M56">
+        <v>40</v>
+      </c>
+      <c r="O56">
+        <f t="shared" si="0"/>
+        <v>587</v>
+      </c>
+      <c r="P56">
+        <f t="shared" si="1"/>
+        <v>627</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>288</v>
+      </c>
+      <c r="D57">
+        <v>220</v>
+      </c>
+      <c r="F57" t="s">
+        <v>351</v>
+      </c>
+      <c r="G57">
+        <v>7</v>
+      </c>
+      <c r="I57" t="s">
+        <v>414</v>
+      </c>
+      <c r="J57">
+        <v>360</v>
+      </c>
+      <c r="L57" t="s">
+        <v>478</v>
+      </c>
+      <c r="M57">
+        <v>40</v>
+      </c>
+      <c r="O57">
+        <f t="shared" si="0"/>
+        <v>587</v>
+      </c>
+      <c r="P57">
+        <f t="shared" si="1"/>
+        <v>627</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>289</v>
+      </c>
+      <c r="D58">
+        <v>280</v>
+      </c>
+      <c r="F58" t="s">
+        <v>352</v>
+      </c>
+      <c r="G58">
+        <v>7</v>
+      </c>
+      <c r="I58" t="s">
+        <v>415</v>
+      </c>
+      <c r="J58">
+        <v>360</v>
+      </c>
+      <c r="L58" t="s">
+        <v>479</v>
+      </c>
+      <c r="M58">
+        <v>30</v>
+      </c>
+      <c r="O58">
+        <f t="shared" si="0"/>
+        <v>647</v>
+      </c>
+      <c r="P58">
+        <f t="shared" si="1"/>
+        <v>677</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>290</v>
+      </c>
+      <c r="D59">
+        <v>280</v>
+      </c>
+      <c r="F59" t="s">
+        <v>353</v>
+      </c>
+      <c r="G59">
+        <v>7</v>
+      </c>
+      <c r="I59" t="s">
+        <v>416</v>
+      </c>
+      <c r="J59">
+        <v>360</v>
+      </c>
+      <c r="L59" t="s">
+        <v>480</v>
+      </c>
+      <c r="M59">
+        <v>30</v>
+      </c>
+      <c r="O59">
+        <f t="shared" si="0"/>
+        <v>647</v>
+      </c>
+      <c r="P59">
+        <f t="shared" si="1"/>
+        <v>677</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>291</v>
+      </c>
+      <c r="D60">
+        <v>10</v>
+      </c>
+      <c r="F60" t="s">
+        <v>354</v>
+      </c>
+      <c r="G60">
+        <v>7</v>
+      </c>
+      <c r="I60" t="s">
+        <v>417</v>
+      </c>
+      <c r="J60">
+        <v>30</v>
+      </c>
+      <c r="L60" t="s">
+        <v>481</v>
+      </c>
+      <c r="M60">
+        <v>90</v>
+      </c>
+      <c r="O60">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="P60">
+        <f t="shared" si="1"/>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>292</v>
+      </c>
+      <c r="D61">
+        <v>300</v>
+      </c>
+      <c r="F61" t="s">
+        <v>355</v>
+      </c>
+      <c r="G61">
+        <v>7</v>
+      </c>
+      <c r="I61" t="s">
+        <v>418</v>
+      </c>
+      <c r="J61">
+        <v>30</v>
+      </c>
+      <c r="L61" t="s">
+        <v>482</v>
+      </c>
+      <c r="M61">
+        <v>30</v>
+      </c>
+      <c r="O61">
         <f t="shared" si="0"/>
         <v>337</v>
       </c>
-      <c r="N21">
+      <c r="P61">
         <f t="shared" si="1"/>
-        <v>397</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>253</v>
-      </c>
-      <c r="B22">
-        <v>10</v>
-      </c>
-      <c r="D22" t="s">
-        <v>320</v>
-      </c>
-      <c r="E22">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>293</v>
+      </c>
+      <c r="D62">
+        <v>300</v>
+      </c>
+      <c r="F62" t="s">
+        <v>356</v>
+      </c>
+      <c r="G62">
         <v>7</v>
       </c>
-      <c r="G22" t="s">
-        <v>383</v>
-      </c>
-      <c r="H22">
+      <c r="I62" t="s">
+        <v>419</v>
+      </c>
+      <c r="J62">
         <v>30</v>
       </c>
-      <c r="J22" t="s">
-        <v>447</v>
-      </c>
-      <c r="K22">
-        <v>40</v>
-      </c>
-      <c r="M22">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="N22">
-        <f t="shared" si="1"/>
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>254</v>
-      </c>
-      <c r="B23">
-        <v>10</v>
-      </c>
-      <c r="D23" t="s">
-        <v>321</v>
-      </c>
-      <c r="E23">
-        <v>7</v>
-      </c>
-      <c r="G23" t="s">
-        <v>384</v>
-      </c>
-      <c r="H23">
+      <c r="L62" t="s">
+        <v>483</v>
+      </c>
+      <c r="M62">
         <v>30</v>
       </c>
-      <c r="J23" t="s">
-        <v>448</v>
-      </c>
-      <c r="K23">
-        <v>40</v>
-      </c>
-      <c r="M23">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="N23">
-        <f t="shared" si="1"/>
-        <v>87</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>255</v>
-      </c>
-      <c r="B24">
-        <v>20</v>
-      </c>
-      <c r="D24" t="s">
-        <v>322</v>
-      </c>
-      <c r="E24">
-        <v>7</v>
-      </c>
-      <c r="G24" t="s">
-        <v>385</v>
-      </c>
-      <c r="H24">
-        <v>60</v>
-      </c>
-      <c r="J24" t="s">
-        <v>449</v>
-      </c>
-      <c r="K24">
-        <v>90</v>
-      </c>
-      <c r="M24">
-        <f t="shared" si="0"/>
-        <v>87</v>
-      </c>
-      <c r="N24">
-        <f t="shared" si="1"/>
-        <v>177</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>256</v>
-      </c>
-      <c r="B25">
-        <v>10</v>
-      </c>
-      <c r="D25" t="s">
-        <v>323</v>
-      </c>
-      <c r="E25">
-        <v>7</v>
-      </c>
-      <c r="G25" t="s">
-        <v>386</v>
-      </c>
-      <c r="H25">
-        <v>30</v>
-      </c>
-      <c r="J25" t="s">
-        <v>450</v>
-      </c>
-      <c r="K25">
-        <v>90</v>
-      </c>
-      <c r="M25">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="N25">
-        <f t="shared" si="1"/>
-        <v>137</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>257</v>
-      </c>
-      <c r="B26">
-        <v>10</v>
-      </c>
-      <c r="D26" t="s">
-        <v>324</v>
-      </c>
-      <c r="E26">
-        <v>7</v>
-      </c>
-      <c r="G26" t="s">
-        <v>387</v>
-      </c>
-      <c r="H26">
-        <v>30</v>
-      </c>
-      <c r="J26" t="s">
-        <v>451</v>
-      </c>
-      <c r="K26">
-        <v>90</v>
-      </c>
-      <c r="M26">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="N26">
-        <f t="shared" si="1"/>
-        <v>137</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>258</v>
-      </c>
-      <c r="B27">
-        <v>10</v>
-      </c>
-      <c r="D27" t="s">
-        <v>325</v>
-      </c>
-      <c r="E27">
-        <v>7</v>
-      </c>
-      <c r="G27" t="s">
-        <v>388</v>
-      </c>
-      <c r="H27">
-        <v>30</v>
-      </c>
-      <c r="J27" t="s">
-        <v>452</v>
-      </c>
-      <c r="K27">
-        <v>90</v>
-      </c>
-      <c r="M27">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="N27">
-        <f t="shared" si="1"/>
-        <v>137</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>259</v>
-      </c>
-      <c r="B28">
-        <v>10</v>
-      </c>
-      <c r="D28" t="s">
-        <v>326</v>
-      </c>
-      <c r="E28">
-        <v>7</v>
-      </c>
-      <c r="G28" t="s">
-        <v>389</v>
-      </c>
-      <c r="H28">
-        <v>30</v>
-      </c>
-      <c r="J28" t="s">
-        <v>453</v>
-      </c>
-      <c r="K28">
-        <v>90</v>
-      </c>
-      <c r="M28">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="N28">
-        <f t="shared" si="1"/>
-        <v>137</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>260</v>
-      </c>
-      <c r="B29">
-        <v>10</v>
-      </c>
-      <c r="D29" t="s">
-        <v>327</v>
-      </c>
-      <c r="E29">
-        <v>7</v>
-      </c>
-      <c r="G29" t="s">
-        <v>390</v>
-      </c>
-      <c r="H29">
-        <v>30</v>
-      </c>
-      <c r="J29" t="s">
-        <v>454</v>
-      </c>
-      <c r="K29">
-        <v>90</v>
-      </c>
-      <c r="M29">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="N29">
-        <f t="shared" si="1"/>
-        <v>137</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>261</v>
-      </c>
-      <c r="B30">
-        <v>10</v>
-      </c>
-      <c r="D30" t="s">
-        <v>328</v>
-      </c>
-      <c r="E30">
-        <v>7</v>
-      </c>
-      <c r="G30" t="s">
-        <v>391</v>
-      </c>
-      <c r="H30">
-        <v>30</v>
-      </c>
-      <c r="J30" t="s">
-        <v>455</v>
-      </c>
-      <c r="K30">
-        <v>90</v>
-      </c>
-      <c r="M30">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="N30">
-        <f t="shared" si="1"/>
-        <v>137</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>262</v>
-      </c>
-      <c r="B31">
-        <v>10</v>
-      </c>
-      <c r="D31" t="s">
-        <v>329</v>
-      </c>
-      <c r="E31">
-        <v>7</v>
-      </c>
-      <c r="G31" t="s">
-        <v>392</v>
-      </c>
-      <c r="H31">
-        <v>30</v>
-      </c>
-      <c r="J31" t="s">
-        <v>456</v>
-      </c>
-      <c r="K31">
-        <v>90</v>
-      </c>
-      <c r="M31">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="N31">
-        <f t="shared" si="1"/>
-        <v>137</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>263</v>
-      </c>
-      <c r="B32">
-        <v>10</v>
-      </c>
-      <c r="D32" t="s">
-        <v>330</v>
-      </c>
-      <c r="E32">
-        <v>7</v>
-      </c>
-      <c r="G32" t="s">
-        <v>393</v>
-      </c>
-      <c r="H32">
-        <v>30</v>
-      </c>
-      <c r="J32" t="s">
-        <v>457</v>
-      </c>
-      <c r="K32">
-        <v>90</v>
-      </c>
-      <c r="M32">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="N32">
-        <f t="shared" si="1"/>
-        <v>137</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>264</v>
-      </c>
-      <c r="B33">
-        <v>10</v>
-      </c>
-      <c r="D33" t="s">
-        <v>331</v>
-      </c>
-      <c r="E33">
-        <v>7</v>
-      </c>
-      <c r="G33" t="s">
-        <v>394</v>
-      </c>
-      <c r="H33">
-        <v>30</v>
-      </c>
-      <c r="J33" t="s">
-        <v>458</v>
-      </c>
-      <c r="K33">
-        <v>90</v>
-      </c>
-      <c r="M33">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="N33">
-        <f t="shared" si="1"/>
-        <v>137</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>265</v>
-      </c>
-      <c r="B34">
-        <v>10</v>
-      </c>
-      <c r="D34" t="s">
-        <v>332</v>
-      </c>
-      <c r="E34">
-        <v>7</v>
-      </c>
-      <c r="G34" t="s">
-        <v>395</v>
-      </c>
-      <c r="H34">
-        <v>30</v>
-      </c>
-      <c r="J34" t="s">
-        <v>459</v>
-      </c>
-      <c r="K34">
-        <v>90</v>
-      </c>
-      <c r="M34">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="N34">
-        <f t="shared" si="1"/>
-        <v>137</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>266</v>
-      </c>
-      <c r="B35">
-        <v>10</v>
-      </c>
-      <c r="D35" t="s">
-        <v>333</v>
-      </c>
-      <c r="E35">
-        <v>7</v>
-      </c>
-      <c r="G35" t="s">
-        <v>396</v>
-      </c>
-      <c r="H35">
-        <v>30</v>
-      </c>
-      <c r="J35" t="s">
-        <v>460</v>
-      </c>
-      <c r="K35">
-        <v>90</v>
-      </c>
-      <c r="M35">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="N35">
-        <f t="shared" si="1"/>
-        <v>137</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>267</v>
-      </c>
-      <c r="B36">
-        <v>10</v>
-      </c>
-      <c r="D36" t="s">
-        <v>334</v>
-      </c>
-      <c r="E36">
-        <v>7</v>
-      </c>
-      <c r="G36" t="s">
-        <v>397</v>
-      </c>
-      <c r="H36">
-        <v>30</v>
-      </c>
-      <c r="J36" t="s">
-        <v>461</v>
-      </c>
-      <c r="K36">
-        <v>90</v>
-      </c>
-      <c r="M36">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="N36">
-        <f t="shared" si="1"/>
-        <v>137</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>268</v>
-      </c>
-      <c r="B37">
-        <v>10</v>
-      </c>
-      <c r="D37" t="s">
-        <v>335</v>
-      </c>
-      <c r="E37">
-        <v>7</v>
-      </c>
-      <c r="G37" t="s">
-        <v>398</v>
-      </c>
-      <c r="H37">
-        <v>30</v>
-      </c>
-      <c r="J37" t="s">
-        <v>462</v>
-      </c>
-      <c r="K37">
-        <v>90</v>
-      </c>
-      <c r="M37">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="N37">
-        <f t="shared" si="1"/>
-        <v>137</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>269</v>
-      </c>
-      <c r="B38">
-        <v>10</v>
-      </c>
-      <c r="D38" t="s">
-        <v>336</v>
-      </c>
-      <c r="E38">
-        <v>7</v>
-      </c>
-      <c r="G38" t="s">
-        <v>399</v>
-      </c>
-      <c r="H38">
-        <v>30</v>
-      </c>
-      <c r="J38" t="s">
-        <v>463</v>
-      </c>
-      <c r="K38">
-        <v>90</v>
-      </c>
-      <c r="M38">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="N38">
-        <f t="shared" si="1"/>
-        <v>137</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>270</v>
-      </c>
-      <c r="B39">
-        <v>10</v>
-      </c>
-      <c r="D39" t="s">
-        <v>337</v>
-      </c>
-      <c r="E39">
-        <v>7</v>
-      </c>
-      <c r="G39" t="s">
-        <v>400</v>
-      </c>
-      <c r="H39">
-        <v>30</v>
-      </c>
-      <c r="J39" t="s">
-        <v>464</v>
-      </c>
-      <c r="K39">
-        <v>90</v>
-      </c>
-      <c r="M39">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="N39">
-        <f t="shared" si="1"/>
-        <v>137</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>271</v>
-      </c>
-      <c r="B40">
-        <v>10</v>
-      </c>
-      <c r="D40" t="s">
-        <v>338</v>
-      </c>
-      <c r="E40">
-        <v>7</v>
-      </c>
-      <c r="G40" t="s">
-        <v>401</v>
-      </c>
-      <c r="H40">
-        <v>30</v>
-      </c>
-      <c r="J40" t="s">
-        <v>465</v>
-      </c>
-      <c r="K40">
-        <v>90</v>
-      </c>
-      <c r="M40">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="N40">
-        <f t="shared" si="1"/>
-        <v>137</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>272</v>
-      </c>
-      <c r="B41">
-        <v>30</v>
-      </c>
-      <c r="D41" t="s">
-        <v>339</v>
-      </c>
-      <c r="E41">
-        <v>7</v>
-      </c>
-      <c r="G41" t="s">
-        <v>402</v>
-      </c>
-      <c r="H41">
-        <v>30</v>
-      </c>
-      <c r="J41" t="s">
-        <v>466</v>
-      </c>
-      <c r="K41">
-        <v>90</v>
-      </c>
-      <c r="M41">
-        <f t="shared" si="0"/>
-        <v>67</v>
-      </c>
-      <c r="N41">
-        <f t="shared" si="1"/>
-        <v>157</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>273</v>
-      </c>
-      <c r="B42">
-        <v>60</v>
-      </c>
-      <c r="D42" t="s">
-        <v>340</v>
-      </c>
-      <c r="E42">
-        <v>7</v>
-      </c>
-      <c r="G42" t="s">
-        <v>403</v>
-      </c>
-      <c r="H42">
-        <v>40</v>
-      </c>
-      <c r="J42" t="s">
-        <v>467</v>
-      </c>
-      <c r="K42">
-        <v>90</v>
-      </c>
-      <c r="M42">
-        <f t="shared" si="0"/>
-        <v>107</v>
-      </c>
-      <c r="N42">
-        <f t="shared" si="1"/>
-        <v>197</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>274</v>
-      </c>
-      <c r="B43">
-        <v>60</v>
-      </c>
-      <c r="D43" t="s">
-        <v>341</v>
-      </c>
-      <c r="E43">
-        <v>7</v>
-      </c>
-      <c r="G43" t="s">
-        <v>404</v>
-      </c>
-      <c r="H43">
-        <v>270</v>
-      </c>
-      <c r="J43" t="s">
-        <v>468</v>
-      </c>
-      <c r="K43">
-        <v>90</v>
-      </c>
-      <c r="M43">
+      <c r="O62">
         <f t="shared" si="0"/>
         <v>337</v>
       </c>
-      <c r="N43">
+      <c r="P62">
         <f t="shared" si="1"/>
-        <v>427</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>275</v>
-      </c>
-      <c r="B44">
-        <v>160</v>
-      </c>
-      <c r="D44" t="s">
-        <v>342</v>
-      </c>
-      <c r="E44">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>294</v>
+      </c>
+      <c r="D63">
+        <v>300</v>
+      </c>
+      <c r="F63" t="s">
+        <v>357</v>
+      </c>
+      <c r="G63">
         <v>7</v>
       </c>
-      <c r="G44" t="s">
-        <v>405</v>
-      </c>
-      <c r="H44">
-        <v>360</v>
-      </c>
-      <c r="J44" t="s">
-        <v>469</v>
-      </c>
-      <c r="K44">
-        <v>90</v>
-      </c>
-      <c r="M44">
-        <f t="shared" si="0"/>
-        <v>527</v>
-      </c>
-      <c r="N44">
-        <f t="shared" si="1"/>
-        <v>617</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>276</v>
-      </c>
-      <c r="B45">
-        <v>160</v>
-      </c>
-      <c r="D45" t="s">
-        <v>343</v>
-      </c>
-      <c r="E45">
-        <v>7</v>
-      </c>
-      <c r="G45" t="s">
-        <v>406</v>
-      </c>
-      <c r="H45">
-        <v>360</v>
-      </c>
-      <c r="J45" t="s">
-        <v>470</v>
-      </c>
-      <c r="K45">
-        <v>90</v>
-      </c>
-      <c r="M45">
-        <f t="shared" si="0"/>
-        <v>527</v>
-      </c>
-      <c r="N45">
-        <f t="shared" si="1"/>
-        <v>617</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>277</v>
-      </c>
-      <c r="B46">
-        <v>160</v>
-      </c>
-      <c r="D46" t="s">
-        <v>344</v>
-      </c>
-      <c r="E46">
-        <v>7</v>
-      </c>
-      <c r="G46" t="s">
-        <v>407</v>
-      </c>
-      <c r="H46">
-        <v>360</v>
-      </c>
-      <c r="J46" t="s">
-        <v>471</v>
-      </c>
-      <c r="K46">
-        <v>90</v>
-      </c>
-      <c r="M46">
-        <f t="shared" si="0"/>
-        <v>527</v>
-      </c>
-      <c r="N46">
-        <f t="shared" si="1"/>
-        <v>617</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>278</v>
-      </c>
-      <c r="B47">
-        <v>150</v>
-      </c>
-      <c r="D47" t="s">
-        <v>345</v>
-      </c>
-      <c r="E47">
-        <v>7</v>
-      </c>
-      <c r="G47" t="s">
-        <v>408</v>
-      </c>
-      <c r="H47">
-        <v>360</v>
-      </c>
-      <c r="J47" t="s">
-        <v>472</v>
-      </c>
-      <c r="K47">
-        <v>40</v>
-      </c>
-      <c r="M47">
-        <f t="shared" si="0"/>
-        <v>517</v>
-      </c>
-      <c r="N47">
-        <f t="shared" si="1"/>
-        <v>557</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>279</v>
-      </c>
-      <c r="B48">
-        <v>150</v>
-      </c>
-      <c r="D48" t="s">
-        <v>346</v>
-      </c>
-      <c r="E48">
-        <v>7</v>
-      </c>
-      <c r="G48" t="s">
-        <v>409</v>
-      </c>
-      <c r="H48">
-        <v>360</v>
-      </c>
-      <c r="J48" t="s">
-        <v>473</v>
-      </c>
-      <c r="K48">
-        <v>40</v>
-      </c>
-      <c r="M48">
-        <f t="shared" si="0"/>
-        <v>517</v>
-      </c>
-      <c r="N48">
-        <f t="shared" si="1"/>
-        <v>557</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>280</v>
-      </c>
-      <c r="B49">
-        <v>150</v>
-      </c>
-      <c r="D49" t="s">
-        <v>347</v>
-      </c>
-      <c r="E49">
-        <v>7</v>
-      </c>
-      <c r="G49" t="s">
-        <v>410</v>
-      </c>
-      <c r="H49">
-        <v>360</v>
-      </c>
-      <c r="J49" t="s">
-        <v>474</v>
-      </c>
-      <c r="K49">
-        <v>40</v>
-      </c>
-      <c r="M49">
-        <f t="shared" si="0"/>
-        <v>517</v>
-      </c>
-      <c r="N49">
-        <f t="shared" si="1"/>
-        <v>557</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>281</v>
-      </c>
-      <c r="B50">
-        <v>20</v>
-      </c>
-      <c r="D50" t="s">
-        <v>348</v>
-      </c>
-      <c r="E50">
-        <v>7</v>
-      </c>
-      <c r="G50" t="s">
-        <v>411</v>
-      </c>
-      <c r="H50">
-        <v>270</v>
-      </c>
-      <c r="J50" t="s">
-        <v>475</v>
-      </c>
-      <c r="K50">
-        <v>90</v>
-      </c>
-      <c r="M50">
-        <f t="shared" si="0"/>
-        <v>297</v>
-      </c>
-      <c r="N50">
-        <f t="shared" si="1"/>
-        <v>387</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>282</v>
-      </c>
-      <c r="B51">
-        <v>20</v>
-      </c>
-      <c r="D51" t="s">
-        <v>349</v>
-      </c>
-      <c r="E51">
-        <v>7</v>
-      </c>
-      <c r="G51" t="s">
-        <v>412</v>
-      </c>
-      <c r="H51">
-        <v>270</v>
-      </c>
-      <c r="J51" t="s">
-        <v>476</v>
-      </c>
-      <c r="K51">
-        <v>90</v>
-      </c>
-      <c r="M51">
-        <f t="shared" si="0"/>
-        <v>297</v>
-      </c>
-      <c r="N51">
-        <f t="shared" si="1"/>
-        <v>387</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>283</v>
-      </c>
-      <c r="B52">
-        <v>20</v>
-      </c>
-      <c r="D52" t="s">
-        <v>350</v>
-      </c>
-      <c r="E52">
-        <v>7</v>
-      </c>
-      <c r="G52" t="s">
-        <v>413</v>
-      </c>
-      <c r="H52">
-        <v>270</v>
-      </c>
-      <c r="J52" t="s">
-        <v>477</v>
-      </c>
-      <c r="K52">
-        <v>90</v>
-      </c>
-      <c r="M52">
-        <f t="shared" si="0"/>
-        <v>297</v>
-      </c>
-      <c r="N52">
-        <f t="shared" si="1"/>
-        <v>387</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>284</v>
-      </c>
-      <c r="B53">
-        <v>290</v>
-      </c>
-      <c r="D53" t="s">
-        <v>351</v>
-      </c>
-      <c r="E53">
-        <v>7</v>
-      </c>
-      <c r="G53" t="s">
-        <v>414</v>
-      </c>
-      <c r="H53">
-        <v>200</v>
-      </c>
-      <c r="J53" t="s">
-        <v>478</v>
-      </c>
-      <c r="K53">
-        <v>50</v>
-      </c>
-      <c r="M53">
-        <f t="shared" si="0"/>
-        <v>497</v>
-      </c>
-      <c r="N53">
-        <f t="shared" si="1"/>
-        <v>547</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>285</v>
-      </c>
-      <c r="B54">
-        <v>230</v>
-      </c>
-      <c r="D54" t="s">
-        <v>352</v>
-      </c>
-      <c r="E54">
-        <v>7</v>
-      </c>
-      <c r="G54" t="s">
-        <v>415</v>
-      </c>
-      <c r="H54">
-        <v>330</v>
-      </c>
-      <c r="J54" t="s">
-        <v>479</v>
-      </c>
-      <c r="K54">
+      <c r="I63" t="s">
+        <v>420</v>
+      </c>
+      <c r="J63">
         <v>30</v>
       </c>
-      <c r="M54">
-        <f t="shared" si="0"/>
-        <v>567</v>
-      </c>
-      <c r="N54">
-        <f t="shared" si="1"/>
-        <v>597</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>286</v>
-      </c>
-      <c r="B55">
-        <v>270</v>
-      </c>
-      <c r="D55" t="s">
-        <v>353</v>
-      </c>
-      <c r="E55">
-        <v>7</v>
-      </c>
-      <c r="G55" t="s">
-        <v>416</v>
-      </c>
-      <c r="H55">
-        <v>360</v>
-      </c>
-      <c r="J55" t="s">
-        <v>480</v>
-      </c>
-      <c r="K55">
-        <v>60</v>
-      </c>
-      <c r="M55">
-        <f t="shared" si="0"/>
-        <v>637</v>
-      </c>
-      <c r="N55">
-        <f t="shared" si="1"/>
-        <v>697</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>287</v>
-      </c>
-      <c r="B56">
-        <v>220</v>
-      </c>
-      <c r="D56" t="s">
-        <v>354</v>
-      </c>
-      <c r="E56">
-        <v>7</v>
-      </c>
-      <c r="G56" t="s">
-        <v>417</v>
-      </c>
-      <c r="H56">
-        <v>360</v>
-      </c>
-      <c r="J56" t="s">
-        <v>481</v>
-      </c>
-      <c r="K56">
-        <v>40</v>
-      </c>
-      <c r="M56">
-        <f t="shared" si="0"/>
-        <v>587</v>
-      </c>
-      <c r="N56">
-        <f t="shared" si="1"/>
-        <v>627</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>288</v>
-      </c>
-      <c r="B57">
-        <v>220</v>
-      </c>
-      <c r="D57" t="s">
-        <v>355</v>
-      </c>
-      <c r="E57">
-        <v>7</v>
-      </c>
-      <c r="G57" t="s">
-        <v>418</v>
-      </c>
-      <c r="H57">
-        <v>360</v>
-      </c>
-      <c r="J57" t="s">
-        <v>482</v>
-      </c>
-      <c r="K57">
-        <v>40</v>
-      </c>
-      <c r="M57">
-        <f t="shared" si="0"/>
-        <v>587</v>
-      </c>
-      <c r="N57">
-        <f t="shared" si="1"/>
-        <v>627</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>289</v>
-      </c>
-      <c r="B58">
-        <v>280</v>
-      </c>
-      <c r="D58" t="s">
-        <v>356</v>
-      </c>
-      <c r="E58">
-        <v>7</v>
-      </c>
-      <c r="G58" t="s">
-        <v>419</v>
-      </c>
-      <c r="H58">
-        <v>360</v>
-      </c>
-      <c r="J58" t="s">
-        <v>483</v>
-      </c>
-      <c r="K58">
+      <c r="L63" t="s">
+        <v>484</v>
+      </c>
+      <c r="M63">
         <v>30</v>
       </c>
-      <c r="M58">
-        <f t="shared" si="0"/>
-        <v>647</v>
-      </c>
-      <c r="N58">
-        <f t="shared" si="1"/>
-        <v>677</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>290</v>
-      </c>
-      <c r="B59">
-        <v>280</v>
-      </c>
-      <c r="D59" t="s">
-        <v>357</v>
-      </c>
-      <c r="E59">
-        <v>7</v>
-      </c>
-      <c r="G59" t="s">
-        <v>420</v>
-      </c>
-      <c r="H59">
-        <v>360</v>
-      </c>
-      <c r="J59" t="s">
-        <v>484</v>
-      </c>
-      <c r="K59">
-        <v>30</v>
-      </c>
-      <c r="M59">
-        <f t="shared" si="0"/>
-        <v>647</v>
-      </c>
-      <c r="N59">
-        <f t="shared" si="1"/>
-        <v>677</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>291</v>
-      </c>
-      <c r="B60">
-        <v>10</v>
-      </c>
-      <c r="D60" t="s">
-        <v>358</v>
-      </c>
-      <c r="E60">
-        <v>7</v>
-      </c>
-      <c r="G60" t="s">
-        <v>421</v>
-      </c>
-      <c r="H60">
-        <v>30</v>
-      </c>
-      <c r="J60" t="s">
-        <v>485</v>
-      </c>
-      <c r="K60">
-        <v>90</v>
-      </c>
-      <c r="M60">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="N60">
-        <f t="shared" si="1"/>
-        <v>137</v>
-      </c>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>292</v>
-      </c>
-      <c r="B61">
-        <v>300</v>
-      </c>
-      <c r="D61" t="s">
-        <v>359</v>
-      </c>
-      <c r="E61">
-        <v>7</v>
-      </c>
-      <c r="G61" t="s">
-        <v>422</v>
-      </c>
-      <c r="H61">
-        <v>30</v>
-      </c>
-      <c r="J61" t="s">
-        <v>486</v>
-      </c>
-      <c r="K61">
-        <v>30</v>
-      </c>
-      <c r="M61">
+      <c r="O63">
         <f t="shared" si="0"/>
         <v>337</v>
       </c>
-      <c r="N61">
+      <c r="P63">
         <f t="shared" si="1"/>
         <v>367</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>293</v>
-      </c>
-      <c r="B62">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>295</v>
+      </c>
+      <c r="D64">
         <v>300</v>
       </c>
-      <c r="D62" t="s">
-        <v>360</v>
-      </c>
-      <c r="E62">
+      <c r="F64" t="s">
+        <v>358</v>
+      </c>
+      <c r="G64">
         <v>7</v>
       </c>
-      <c r="G62" t="s">
-        <v>423</v>
-      </c>
-      <c r="H62">
+      <c r="I64" t="s">
+        <v>421</v>
+      </c>
+      <c r="J64">
         <v>30</v>
       </c>
-      <c r="J62" t="s">
-        <v>487</v>
-      </c>
-      <c r="K62">
+      <c r="L64" t="s">
+        <v>485</v>
+      </c>
+      <c r="M64">
         <v>30</v>
       </c>
-      <c r="M62">
+      <c r="O64">
         <f t="shared" si="0"/>
         <v>337</v>
       </c>
-      <c r="N62">
+      <c r="P64">
         <f t="shared" si="1"/>
         <v>367</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>294</v>
-      </c>
-      <c r="B63">
-        <v>300</v>
-      </c>
-      <c r="D63" t="s">
-        <v>361</v>
-      </c>
-      <c r="E63">
-        <v>7</v>
-      </c>
-      <c r="G63" t="s">
-        <v>424</v>
-      </c>
-      <c r="H63">
-        <v>30</v>
-      </c>
-      <c r="J63" t="s">
-        <v>488</v>
-      </c>
-      <c r="K63">
-        <v>30</v>
-      </c>
-      <c r="M63">
-        <f t="shared" si="0"/>
-        <v>337</v>
-      </c>
-      <c r="N63">
-        <f t="shared" si="1"/>
-        <v>367</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>295</v>
-      </c>
-      <c r="B64">
-        <v>300</v>
-      </c>
-      <c r="D64" t="s">
-        <v>362</v>
-      </c>
-      <c r="E64">
-        <v>7</v>
-      </c>
-      <c r="G64" t="s">
-        <v>425</v>
-      </c>
-      <c r="H64">
-        <v>30</v>
-      </c>
-      <c r="J64" t="s">
-        <v>489</v>
-      </c>
-      <c r="K64">
-        <v>30</v>
-      </c>
-      <c r="M64">
-        <f t="shared" si="0"/>
-        <v>337</v>
-      </c>
-      <c r="N64">
-        <f t="shared" si="1"/>
-        <v>367</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>296</v>
-      </c>
-      <c r="B65">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>297</v>
-      </c>
-      <c r="B66">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>298</v>
-      </c>
-      <c r="B67">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>299</v>
-      </c>
-      <c r="B68">
-        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>